<commit_message>
This commit includes the following updates - Change trim threshold to 0.4998 in preprocessor, utils, and evaluation notebook - Update documentation - Update tests
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-self-summary-with-xlsx-output/output/model_comparison_eval_short.xlsx
+++ b/tests/data/experiments/lr-self-summary-with-xlsx-output/output/model_comparison_eval_short.xlsx
@@ -1,37 +1,108 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>SMD (rounded)</t>
+  </si>
+  <si>
+    <t>adj_agr (rounded)</t>
+  </si>
+  <si>
+    <t>corr</t>
+  </si>
+  <si>
+    <t>exact_agr (rounded)</t>
+  </si>
+  <si>
+    <t>h_mean</t>
+  </si>
+  <si>
+    <t>h_sd</t>
+  </si>
+  <si>
+    <t>kappa (rounded)</t>
+  </si>
+  <si>
+    <t>sys_mean</t>
+  </si>
+  <si>
+    <t>sys_mean (rounded)</t>
+  </si>
+  <si>
+    <t>sys_sd</t>
+  </si>
+  <si>
+    <t>sys_sd (rounded)</t>
+  </si>
+  <si>
+    <t>system score type</t>
+  </si>
+  <si>
+    <t>truncation range</t>
+  </si>
+  <si>
+    <t>wtkappa (rounded)</t>
+  </si>
+  <si>
+    <t>lr_subgroups</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>[0.5002, 6.4998000000000005]</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,26 +117,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -353,307 +433,247 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>R2</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>RMSE</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>SMD</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>SMD (rounded)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>adj_agr (rounded)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>corr</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>exact_agr (rounded)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>h_mean</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>h_sd</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>kappa (rounded)</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>sys_mean</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>sys_mean (rounded)</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>sys_sd</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>sys_sd (rounded)</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>system score type</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>truncation range</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>wtkappa (rounded)</t>
-        </is>
+    <row r="1" spans="1:19">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>lr_subgroups</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="2" spans="1:19">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
         <v>200</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>0.5493203316759259</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>0.6189327249996263</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>0.02324751973534952</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>-0.01054416404922412</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>99</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>0.7801773732608189</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>64</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2">
         <v>3.5</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2">
         <v>0.9242680113386592</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2">
         <v>0.4694178334561533</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2">
         <v>3.521731815875492</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2">
         <v>3.49</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2">
         <v>0.9452175731243876</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P2">
         <v>0.97191723700009</v>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>scale</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>[0.50002, 6.49998]</t>
-        </is>
-      </c>
-      <c r="S2" t="n">
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2">
         <v>0.782122905027933</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>lr_subgroups</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:19">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
         <v>200</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>0.5493203316759259</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>0.6189327249996263</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>0.02324751973534952</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>-0.01054416404922412</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>99</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>0.7801773732608189</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3">
         <v>64</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J3">
         <v>3.5</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3">
         <v>0.9242680113386592</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3">
         <v>0.4694178334561533</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M3">
         <v>3.521731815875492</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N3">
         <v>3.49</v>
       </c>
-      <c r="O3" t="n">
+      <c r="O3">
         <v>0.9452175731243876</v>
       </c>
-      <c r="P3" t="n">
+      <c r="P3">
         <v>0.97191723700009</v>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>scale</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>[0.50002, 6.49998]</t>
-        </is>
-      </c>
-      <c r="S3" t="n">
+      <c r="Q3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3">
         <v>0.782122905027933</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>lr_subgroups</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:19">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
         <v>200</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>0.5493203316759259</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>0.6189327249996263</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>0.02324751973534952</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>-0.01054416404922412</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>99</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>0.7801773732608189</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4">
         <v>64</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J4">
         <v>3.5</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4">
         <v>0.9242680113386592</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L4">
         <v>0.4694178334561533</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M4">
         <v>3.521731815875492</v>
       </c>
-      <c r="N4" t="n">
+      <c r="N4">
         <v>3.49</v>
       </c>
-      <c r="O4" t="n">
+      <c r="O4">
         <v>0.9452175731243876</v>
       </c>
-      <c r="P4" t="n">
+      <c r="P4">
         <v>0.97191723700009</v>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>scale</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>[0.50002, 6.49998]</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
+      <c r="Q4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4">
         <v>0.782122905027933</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>